<commit_message>
Up-to-date : ready to turn in
</commit_message>
<xml_diff>
--- a/TeamWeeklyReport.xlsx
+++ b/TeamWeeklyReport.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\l3ryc\Documents\School\College\CS 499\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FF95448-99D8-4E8E-B9EE-768FB7BCB925}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37AA788B-4B6C-4F67-A082-125332661EB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-4815" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Members List" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
     <sheet name="Problem Reports" sheetId="12" r:id="rId12"/>
     <sheet name="Lists" sheetId="13" r:id="rId13"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" refMode="R1C1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -339,7 +339,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="328">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="335">
   <si>
     <t>Name</t>
   </si>
@@ -398,9 +398,6 @@
     <t>None</t>
   </si>
   <si>
-    <t>None, so far, but I do expect this to be populated</t>
-  </si>
-  <si>
     <t>Bryce</t>
   </si>
   <si>
@@ -560,9 +557,6 @@
     <t>AI-04</t>
   </si>
   <si>
-    <t>AI-05</t>
-  </si>
-  <si>
     <t>Epic ID</t>
   </si>
   <si>
@@ -917,9 +911,6 @@
     <t>Actual Complete Date</t>
   </si>
   <si>
-    <t>Assigne to</t>
-  </si>
-  <si>
     <t>Verified by</t>
   </si>
   <si>
@@ -1323,6 +1314,36 @@
   </si>
   <si>
     <t>https://docs.google.com/document/d/1FiHYzerAfcxR32JLNc62Wz9frG3MbLFIbiTUE0AMYsA/edit?usp=sharing</t>
+  </si>
+  <si>
+    <t>Time (hrs)</t>
+  </si>
+  <si>
+    <t>Begin React Training, 4.1,5.1</t>
+  </si>
+  <si>
+    <t>Library Research, 5.2,5.4</t>
+  </si>
+  <si>
+    <t>Begin React Training, 6.1,6.2</t>
+  </si>
+  <si>
+    <t>1.1,1.2 Research</t>
+  </si>
+  <si>
+    <t>Begin learning react and refresh yourself on sections 4.1 and 5.1</t>
+  </si>
+  <si>
+    <t>Begin learning react and refresh yourself on sections 6.1 and 6.2</t>
+  </si>
+  <si>
+    <t>Consider different python libraries to aid in discrete math and resfresh yourself on sections 5.2 and 5.4</t>
+  </si>
+  <si>
+    <t>Refresh yourself on sections 1.1 and 1.2, do preliminary code work on section 1.1</t>
+  </si>
+  <si>
+    <t>moving to Philly in May, this does not cause problems now, but may in the future.</t>
   </si>
 </sst>
 </file>
@@ -1332,7 +1353,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[&lt;=9999999]###\-####;\(###\)\ ###\-####"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1354,6 +1375,19 @@
       <sz val="11"/>
       <color theme="10"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1377,13 +1411,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1396,6 +1429,11 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1614,9 +1652,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J14" sqref="J14"/>
+      <selection pane="bottomLeft" activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1710,19 +1748,19 @@
       <c r="J2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="K2" s="5" t="s">
-        <v>19</v>
+      <c r="K2" s="15" t="s">
+        <v>334</v>
       </c>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" s="3" t="s">
         <v>21</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>22</v>
       </c>
       <c r="D3" s="4">
         <v>8652303400</v>
@@ -1731,62 +1769,62 @@
         <v>13</v>
       </c>
       <c r="F3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="H3" s="2" t="s">
         <v>24</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>25</v>
       </c>
       <c r="I3" s="2" t="e">
         <f>NA()</f>
         <v>#N/A</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B4" s="2"/>
-      <c r="C4" s="11" t="s">
-        <v>322</v>
+      <c r="C4" s="10" t="s">
+        <v>319</v>
       </c>
       <c r="D4" s="4">
         <v>2054170106</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="F4" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G4" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="G4" s="6" t="s">
+      <c r="H4" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="I4" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J4" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="H4" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="I4" s="6" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="J4" s="6" t="s">
+      <c r="K4" s="5" t="s">
         <v>30</v>
-      </c>
-      <c r="K4" s="6" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B5" s="2"/>
-      <c r="C5" s="11" t="s">
-        <v>323</v>
+      <c r="C5" s="10" t="s">
+        <v>320</v>
       </c>
       <c r="D5" s="4">
         <v>2054410261</v>
@@ -1795,23 +1833,23 @@
         <v>13</v>
       </c>
       <c r="F5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G5" t="s">
         <v>28</v>
       </c>
-      <c r="G5" t="s">
-        <v>29</v>
-      </c>
       <c r="H5" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="I5" t="e">
         <f>NA()</f>
         <v>#N/A</v>
       </c>
       <c r="J5" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="K5" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.25">
@@ -4844,27 +4882,27 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>236</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>238</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="E2" s="2">
         <f t="shared" ref="E2:E8" si="0">C2*D2</f>
@@ -4873,7 +4911,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="E3" s="2">
         <f t="shared" si="0"/>
@@ -4882,7 +4920,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="E4" s="2">
         <f t="shared" si="0"/>
@@ -4891,7 +4929,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="E5" s="2">
         <f t="shared" si="0"/>
@@ -4900,7 +4938,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="E6" s="2">
         <f t="shared" si="0"/>
@@ -4909,7 +4947,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="E7" s="2">
         <f t="shared" si="0"/>
@@ -4918,7 +4956,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="E8" s="2">
         <f t="shared" si="0"/>
@@ -5930,104 +5968,104 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
-        <v>247</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>248</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="E1" s="7" t="s">
-        <v>249</v>
-      </c>
-      <c r="F1" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
-      <c r="K1" s="7"/>
-      <c r="L1" s="7"/>
-      <c r="M1" s="7"/>
-      <c r="N1" s="7"/>
-      <c r="O1" s="7"/>
-      <c r="P1" s="7"/>
-      <c r="Q1" s="7"/>
-      <c r="R1" s="7"/>
-      <c r="S1" s="7"/>
-      <c r="T1" s="7"/>
-      <c r="U1" s="7"/>
-      <c r="V1" s="7"/>
-      <c r="W1" s="7"/>
-      <c r="X1" s="7"/>
-      <c r="Y1" s="7"/>
-      <c r="Z1" s="7"/>
+      <c r="A1" s="6" t="s">
+        <v>244</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>245</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>246</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
+      <c r="M1" s="6"/>
+      <c r="N1" s="6"/>
+      <c r="O1" s="6"/>
+      <c r="P1" s="6"/>
+      <c r="Q1" s="6"/>
+      <c r="R1" s="6"/>
+      <c r="S1" s="6"/>
+      <c r="T1" s="6"/>
+      <c r="U1" s="6"/>
+      <c r="V1" s="6"/>
+      <c r="W1" s="6"/>
+      <c r="X1" s="6"/>
+      <c r="Y1" s="6"/>
+      <c r="Z1" s="6"/>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
@@ -7055,50 +7093,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="6" t="s">
+        <v>256</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>257</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>246</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>258</v>
+      </c>
+      <c r="G1" s="6" t="s">
         <v>259</v>
       </c>
-      <c r="B1" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>260</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="E1" s="7" t="s">
-        <v>249</v>
-      </c>
-      <c r="F1" s="7" t="s">
-        <v>261</v>
-      </c>
-      <c r="G1" s="7" t="s">
-        <v>262</v>
-      </c>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
-      <c r="K1" s="7"/>
-      <c r="L1" s="7"/>
-      <c r="M1" s="7"/>
-      <c r="N1" s="7"/>
-      <c r="O1" s="7"/>
-      <c r="P1" s="7"/>
-      <c r="Q1" s="7"/>
-      <c r="R1" s="7"/>
-      <c r="S1" s="7"/>
-      <c r="T1" s="7"/>
-      <c r="U1" s="7"/>
-      <c r="V1" s="7"/>
-      <c r="W1" s="7"/>
-      <c r="X1" s="7"/>
-      <c r="Y1" s="7"/>
-      <c r="Z1" s="7"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
+      <c r="M1" s="6"/>
+      <c r="N1" s="6"/>
+      <c r="O1" s="6"/>
+      <c r="P1" s="6"/>
+      <c r="Q1" s="6"/>
+      <c r="R1" s="6"/>
+      <c r="S1" s="6"/>
+      <c r="T1" s="6"/>
+      <c r="U1" s="6"/>
+      <c r="V1" s="6"/>
+      <c r="W1" s="6"/>
+      <c r="X1" s="6"/>
+      <c r="Y1" s="6"/>
+      <c r="Z1" s="6"/>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
@@ -7106,7 +7144,7 @@
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
@@ -7114,7 +7152,7 @@
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
@@ -7122,7 +7160,7 @@
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
@@ -7130,7 +7168,7 @@
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
@@ -7138,7 +7176,7 @@
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
@@ -7146,7 +7184,7 @@
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
@@ -7154,7 +7192,7 @@
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
@@ -7162,7 +7200,7 @@
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
@@ -7170,7 +7208,7 @@
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
@@ -7178,7 +7216,7 @@
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
@@ -7186,7 +7224,7 @@
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
@@ -7194,7 +7232,7 @@
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
@@ -7202,7 +7240,7 @@
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
@@ -7210,7 +7248,7 @@
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
@@ -7218,7 +7256,7 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
@@ -7226,7 +7264,7 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
@@ -7234,7 +7272,7 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
@@ -7242,7 +7280,7 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
@@ -7250,7 +7288,7 @@
     </row>
     <row r="21" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
@@ -7258,7 +7296,7 @@
     </row>
     <row r="22" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
@@ -7266,7 +7304,7 @@
     </row>
     <row r="23" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
@@ -7274,49 +7312,49 @@
     </row>
     <row r="24" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="D24" s="2"/>
       <c r="F24" s="2"/>
     </row>
     <row r="25" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="D25" s="2"/>
       <c r="F25" s="2"/>
     </row>
     <row r="26" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="D26" s="2"/>
       <c r="F26" s="2"/>
     </row>
     <row r="27" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="D27" s="2"/>
       <c r="F27" s="2"/>
     </row>
     <row r="28" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="D28" s="2"/>
       <c r="F28" s="2"/>
     </row>
     <row r="29" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="D29" s="2"/>
       <c r="F29" s="2"/>
     </row>
     <row r="30" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="D30" s="2"/>
       <c r="F30" s="2"/>
@@ -8342,25 +8380,25 @@
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>292</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>293</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>294</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>295</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>296</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>297</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>298</v>
       </c>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
@@ -8383,25 +8421,25 @@
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>300</v>
-      </c>
-      <c r="D2" s="9">
+        <v>297</v>
+      </c>
+      <c r="D2" s="8">
         <v>44572</v>
       </c>
-      <c r="E2" s="9">
+      <c r="E2" s="8">
         <v>44680</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="H2" s="2" t="str">
         <f>'Members List'!A2</f>
@@ -8410,19 +8448,19 @@
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>302</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="G3" s="2" t="s">
         <v>303</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>304</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>305</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>306</v>
       </c>
       <c r="H3" s="2" t="str">
         <f>'Members List'!A3</f>
@@ -8431,19 +8469,19 @@
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="G4" s="2" t="s">
         <v>307</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>308</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>309</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>310</v>
       </c>
       <c r="H4" s="2" t="str">
         <f>'Members List'!A4</f>
@@ -8452,19 +8490,19 @@
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>309</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="F5" s="2" t="s">
         <v>311</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="G5" s="2" t="s">
         <v>312</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>313</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>314</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>315</v>
       </c>
       <c r="H5" s="2" t="str">
         <f>'Members List'!A5</f>
@@ -8473,10 +8511,10 @@
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="H6" s="2">
         <f>'Members List'!A6</f>
@@ -8485,23 +8523,23 @@
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="H9" s="2" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -9499,7 +9537,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D19" sqref="D19"/>
+      <selection pane="bottomRight" activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -9510,114 +9548,114 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="C1" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="D1" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="E1" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="F1" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="G1" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="H1" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="I1" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="J1" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="K1" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="K1" s="7" t="s">
+      <c r="L1" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="L1" s="7" t="s">
+      <c r="M1" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="M1" s="7" t="s">
+      <c r="N1" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="N1" s="7" t="s">
+      <c r="O1" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="O1" s="7" t="s">
+      <c r="P1" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="P1" s="7" t="s">
+      <c r="Q1" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="Q1" s="7" t="s">
+      <c r="R1" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="R1" s="7" t="s">
+      <c r="S1" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="S1" s="7" t="s">
+      <c r="T1" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="T1" s="7" t="s">
+      <c r="U1" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="U1" s="7" t="s">
+      <c r="V1" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="V1" s="7" t="s">
+      <c r="W1" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="W1" s="7" t="s">
+      <c r="X1" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="X1" s="7" t="s">
+      <c r="Y1" s="6"/>
+      <c r="Z1" s="6"/>
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="Y1" s="7"/>
-      <c r="Z1" s="7"/>
-    </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="B2" s="8">
+      <c r="B2" s="7">
         <v>44572</v>
       </c>
-      <c r="C2" s="8">
+      <c r="C2" s="7">
         <v>44574</v>
       </c>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="8"/>
-      <c r="K2" s="8"/>
-      <c r="L2" s="8"/>
-      <c r="M2" s="8"/>
-      <c r="N2" s="8"/>
-      <c r="O2" s="8"/>
-      <c r="P2" s="8"/>
-      <c r="Q2" s="8"/>
-      <c r="R2" s="8"/>
-      <c r="S2" s="8"/>
-      <c r="T2" s="8"/>
-      <c r="U2" s="8"/>
-      <c r="V2" s="8"/>
-      <c r="W2" s="8"/>
-      <c r="X2" s="8"/>
-      <c r="Y2" s="7"/>
-      <c r="Z2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="7"/>
+      <c r="L2" s="7"/>
+      <c r="M2" s="7"/>
+      <c r="N2" s="7"/>
+      <c r="O2" s="7"/>
+      <c r="P2" s="7"/>
+      <c r="Q2" s="7"/>
+      <c r="R2" s="7"/>
+      <c r="S2" s="7"/>
+      <c r="T2" s="7"/>
+      <c r="U2" s="7"/>
+      <c r="V2" s="7"/>
+      <c r="W2" s="7"/>
+      <c r="X2" s="7"/>
+      <c r="Y2" s="6"/>
+      <c r="Z2" s="6"/>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="str">
@@ -9625,10 +9663,10 @@
         <v>Sam</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
@@ -9658,10 +9696,10 @@
         <v>Bryce</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
@@ -9691,10 +9729,10 @@
         <v>Pierre</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
@@ -9724,10 +9762,10 @@
         <v>Chaz</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
@@ -9782,13 +9820,24 @@
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>60</v>
-      </c>
       <c r="C8" t="s">
-        <v>327</v>
+        <v>324</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="11" t="s">
+        <v>325</v>
+      </c>
+      <c r="B9">
+        <v>0.5</v>
+      </c>
+      <c r="C9">
+        <v>1.5</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -10794,9 +10843,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomLeft" activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -10814,28 +10863,28 @@
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>67</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>68</v>
       </c>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
@@ -10858,41 +10907,94 @@
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="2"/>
+        <v>68</v>
+      </c>
+      <c r="B2" s="12">
+        <v>44574</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="D2" s="8"/>
+      <c r="E2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>326</v>
+      </c>
+      <c r="G2" s="11" t="s">
+        <v>330</v>
+      </c>
+      <c r="H2" s="13"/>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="B3" s="9"/>
-      <c r="C3" s="2"/>
+        <v>69</v>
+      </c>
+      <c r="B3" s="8">
+        <v>44574</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>297</v>
+      </c>
       <c r="D3" s="2"/>
+      <c r="E3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>327</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>332</v>
+      </c>
+      <c r="H3" s="11"/>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
+        <v>70</v>
+      </c>
+      <c r="B4" s="12">
+        <v>44574</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>297</v>
+      </c>
       <c r="D4" s="2"/>
+      <c r="E4" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>328</v>
+      </c>
+      <c r="G4" s="11" t="s">
+        <v>331</v>
+      </c>
+      <c r="H4" s="11"/>
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
+        <v>71</v>
+      </c>
+      <c r="B5" s="12">
+        <v>44574</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>297</v>
+      </c>
       <c r="D5" s="2"/>
+      <c r="E5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>329</v>
+      </c>
+      <c r="G5" s="11" t="s">
+        <v>333</v>
+      </c>
+      <c r="H5" s="11"/>
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>73</v>
-      </c>
+      <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
@@ -11977,7 +12079,7 @@
           <x14:formula1>
             <xm:f>'Members List'!$A$2:$A$6</xm:f>
           </x14:formula1>
-          <xm:sqref>E2</xm:sqref>
+          <xm:sqref>E2:E5</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -12004,13 +12106,13 @@
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>74</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>76</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -12038,67 +12140,67 @@
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -13110,25 +13212,25 @@
   <sheetData>
     <row r="1" spans="1:26" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="E1" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="G1" s="9" t="s">
         <v>93</v>
-      </c>
-      <c r="F1" s="10" t="s">
-        <v>94</v>
-      </c>
-      <c r="G1" s="10" t="s">
-        <v>95</v>
       </c>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
@@ -13153,7 +13255,7 @@
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
       <c r="B2" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
@@ -13161,7 +13263,7 @@
     <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
@@ -13169,7 +13271,7 @@
     <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
@@ -13177,7 +13279,7 @@
     <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
       <c r="B5" s="2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
@@ -13185,7 +13287,7 @@
     <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
@@ -13193,7 +13295,7 @@
     <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
@@ -13201,7 +13303,7 @@
     <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
@@ -13209,7 +13311,7 @@
     <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
@@ -13217,7 +13319,7 @@
     <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
@@ -13225,7 +13327,7 @@
     <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
@@ -13233,7 +13335,7 @@
     <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
@@ -13241,7 +13343,7 @@
     <row r="13" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
@@ -13249,7 +13351,7 @@
     <row r="14" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
@@ -13257,7 +13359,7 @@
     <row r="15" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="2" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
@@ -13265,7 +13367,7 @@
     <row r="16" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="2" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
@@ -13273,7 +13375,7 @@
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
@@ -13281,7 +13383,7 @@
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
       <c r="B18" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
@@ -13289,7 +13391,7 @@
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
       <c r="B19" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
@@ -13297,7 +13399,7 @@
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
       <c r="B20" s="2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
@@ -13305,7 +13407,7 @@
     <row r="21" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
       <c r="B21" s="2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
@@ -13313,7 +13415,7 @@
     <row r="22" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
       <c r="B22" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
@@ -13321,7 +13423,7 @@
     <row r="23" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
       <c r="B23" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
@@ -13329,7 +13431,7 @@
     <row r="24" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
       <c r="B24" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
@@ -13337,7 +13439,7 @@
     <row r="25" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
       <c r="B25" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
@@ -13345,7 +13447,7 @@
     <row r="26" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
       <c r="B26" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
@@ -13353,7 +13455,7 @@
     <row r="27" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
       <c r="B27" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
@@ -13361,7 +13463,7 @@
     <row r="28" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
       <c r="B28" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
@@ -13369,7 +13471,7 @@
     <row r="29" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2"/>
       <c r="B29" s="2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
@@ -13377,7 +13479,7 @@
     <row r="30" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2"/>
       <c r="B30" s="2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
@@ -14393,13 +14495,13 @@
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>125</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>127</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -14427,47 +14529,47 @@
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -15475,22 +15577,22 @@
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>140</v>
-      </c>
       <c r="F1" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
@@ -15516,238 +15618,238 @@
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
       <c r="B2" s="2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="F2" s="2"/>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" s="2" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="F3" s="2"/>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" s="2" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="F4" s="2"/>
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
       <c r="B5" s="2" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="F5" s="2"/>
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="F6" s="2"/>
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" s="2" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="F7" s="2"/>
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F8" s="2"/>
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="2" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="F9" s="2"/>
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="2" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="F10" s="2"/>
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="2" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F11" s="2"/>
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="2" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="F12" s="2"/>
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="F13" s="2"/>
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="2" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="F14" s="2"/>
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="2" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="F15" s="2"/>
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="2" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F16" s="2"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" s="2" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="F17" s="2"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
       <c r="B18" s="2" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="F18" s="2"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
       <c r="B19" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="F19" s="2"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
       <c r="B20" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="F20" s="2"/>
     </row>
     <row r="21" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
       <c r="B21" s="2" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="F21" s="2"/>
     </row>
     <row r="22" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
       <c r="B22" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="F22" s="2"/>
     </row>
     <row r="23" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
       <c r="B23" s="2" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="F23" s="2"/>
     </row>
     <row r="24" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
       <c r="B24" s="2" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="F24" s="2"/>
     </row>
     <row r="25" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
       <c r="B25" s="2" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="F25" s="2"/>
     </row>
     <row r="26" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
       <c r="B26" s="2" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="F26" s="2"/>
     </row>
     <row r="27" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
       <c r="B27" s="2" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="F27" s="2"/>
     </row>
     <row r="28" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
       <c r="B28" s="2" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="F28" s="2"/>
     </row>
     <row r="29" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2"/>
       <c r="B29" s="2" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="F29" s="2"/>
     </row>
     <row r="30" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2"/>
       <c r="B30" s="2" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="F30" s="2"/>
     </row>
     <row r="31" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="2"/>
       <c r="B31" s="2" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="F31" s="2"/>
     </row>
     <row r="32" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="2"/>
       <c r="B32" s="2" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="F32" s="2"/>
     </row>
     <row r="33" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="2"/>
       <c r="B33" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="F33" s="2"/>
     </row>
     <row r="34" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="2"/>
       <c r="B34" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="F34" s="2"/>
     </row>
     <row r="35" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="2"/>
       <c r="B35" s="2" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="F35" s="2"/>
     </row>
@@ -16754,67 +16856,67 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -17809,7 +17911,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomLeft" activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -17826,25 +17928,25 @@
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>190</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>193</v>
       </c>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
@@ -17868,529 +17970,546 @@
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="B2" s="9">
+        <v>191</v>
+      </c>
+      <c r="B2" s="8">
         <v>44572</v>
       </c>
-      <c r="C2" s="9">
+      <c r="C2" s="8">
         <f>B2</f>
         <v>44572</v>
       </c>
-      <c r="D2" s="9">
-        <v>44578</v>
+      <c r="D2" s="8">
+        <v>44577</v>
+      </c>
+      <c r="E2" s="13">
+        <f>D2</f>
+        <v>44577</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="D3" s="9">
+        <v>193</v>
+      </c>
+      <c r="D3" s="8">
         <f t="shared" ref="D3:D17" si="0">D2+7</f>
-        <v>44585</v>
+        <v>44584</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="D4" s="9">
+        <v>194</v>
+      </c>
+      <c r="D4" s="8">
         <f t="shared" si="0"/>
-        <v>44592</v>
+        <v>44591</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="D5" s="9">
+        <v>195</v>
+      </c>
+      <c r="D5" s="8">
         <f t="shared" si="0"/>
-        <v>44599</v>
+        <v>44598</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="D6" s="9">
+        <v>196</v>
+      </c>
+      <c r="D6" s="8">
         <f t="shared" si="0"/>
-        <v>44606</v>
+        <v>44605</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="D7" s="9">
+        <v>197</v>
+      </c>
+      <c r="D7" s="8">
         <f t="shared" si="0"/>
-        <v>44613</v>
+        <v>44612</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="D8" s="9">
+        <v>198</v>
+      </c>
+      <c r="D8" s="8">
         <f t="shared" si="0"/>
-        <v>44620</v>
+        <v>44619</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="D9" s="9">
+        <v>199</v>
+      </c>
+      <c r="D9" s="8">
         <f t="shared" si="0"/>
-        <v>44627</v>
+        <v>44626</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="D10" s="9">
+        <v>200</v>
+      </c>
+      <c r="D10" s="8">
         <f t="shared" si="0"/>
-        <v>44634</v>
+        <v>44633</v>
       </c>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>204</v>
-      </c>
-      <c r="D11" s="9">
+        <v>201</v>
+      </c>
+      <c r="D11" s="8">
         <f t="shared" si="0"/>
-        <v>44641</v>
+        <v>44640</v>
       </c>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>205</v>
-      </c>
-      <c r="D12" s="9">
+        <v>202</v>
+      </c>
+      <c r="D12" s="8">
         <f t="shared" si="0"/>
-        <v>44648</v>
+        <v>44647</v>
       </c>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>206</v>
-      </c>
-      <c r="D13" s="9">
+        <v>203</v>
+      </c>
+      <c r="D13" s="8">
         <f t="shared" si="0"/>
-        <v>44655</v>
+        <v>44654</v>
       </c>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>207</v>
-      </c>
-      <c r="D14" s="9">
+        <v>204</v>
+      </c>
+      <c r="D14" s="8">
         <f t="shared" si="0"/>
-        <v>44662</v>
+        <v>44661</v>
       </c>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>208</v>
-      </c>
-      <c r="D15" s="9">
+        <v>205</v>
+      </c>
+      <c r="D15" s="8">
         <f t="shared" si="0"/>
-        <v>44669</v>
+        <v>44668</v>
       </c>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>209</v>
-      </c>
-      <c r="D16" s="9">
+        <v>206</v>
+      </c>
+      <c r="D16" s="8">
         <f t="shared" si="0"/>
-        <v>44676</v>
+        <v>44675</v>
       </c>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>210</v>
-      </c>
-      <c r="D17" s="9">
+        <v>207</v>
+      </c>
+      <c r="D17" s="8">
         <f t="shared" si="0"/>
-        <v>44683</v>
+        <v>44682</v>
       </c>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D18" s="9"/>
+      <c r="D18" s="8"/>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>211</v>
-      </c>
-      <c r="D19" s="9">
-        <v>44578</v>
-      </c>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
+        <v>208</v>
+      </c>
+      <c r="B19" s="13">
+        <v>44572</v>
+      </c>
+      <c r="C19" s="13">
+        <v>44572</v>
+      </c>
+      <c r="D19" s="8">
+        <v>44577</v>
+      </c>
+      <c r="E19" s="13">
+        <v>44577</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>192</v>
+      </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>212</v>
-      </c>
-      <c r="D20" s="9">
+        <v>209</v>
+      </c>
+      <c r="D20" s="8">
         <f t="shared" ref="D20:D34" si="1">D19+7</f>
-        <v>44585</v>
+        <v>44584</v>
       </c>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
     </row>
     <row r="21" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>213</v>
-      </c>
-      <c r="D21" s="9">
+        <v>210</v>
+      </c>
+      <c r="D21" s="8">
         <f t="shared" si="1"/>
-        <v>44592</v>
+        <v>44591</v>
       </c>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
     </row>
     <row r="22" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="D22" s="9">
+        <v>211</v>
+      </c>
+      <c r="D22" s="8">
         <f t="shared" si="1"/>
-        <v>44599</v>
+        <v>44598</v>
       </c>
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
     </row>
     <row r="23" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>215</v>
-      </c>
-      <c r="D23" s="9">
+        <v>212</v>
+      </c>
+      <c r="D23" s="8">
         <f t="shared" si="1"/>
-        <v>44606</v>
+        <v>44605</v>
       </c>
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
     </row>
     <row r="24" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="D24" s="9">
+        <v>213</v>
+      </c>
+      <c r="D24" s="8">
         <f t="shared" si="1"/>
-        <v>44613</v>
+        <v>44612</v>
       </c>
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
     </row>
     <row r="25" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>217</v>
-      </c>
-      <c r="D25" s="9">
+        <v>214</v>
+      </c>
+      <c r="D25" s="8">
         <f t="shared" si="1"/>
-        <v>44620</v>
+        <v>44619</v>
       </c>
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
     </row>
     <row r="26" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>218</v>
-      </c>
-      <c r="D26" s="9">
+        <v>215</v>
+      </c>
+      <c r="D26" s="8">
         <f t="shared" si="1"/>
-        <v>44627</v>
+        <v>44626</v>
       </c>
       <c r="F26" s="2"/>
       <c r="G26" s="2"/>
     </row>
     <row r="27" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>219</v>
-      </c>
-      <c r="D27" s="9">
+        <v>216</v>
+      </c>
+      <c r="D27" s="8">
         <f t="shared" si="1"/>
-        <v>44634</v>
+        <v>44633</v>
       </c>
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
     </row>
     <row r="28" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>220</v>
-      </c>
-      <c r="D28" s="9">
+        <v>217</v>
+      </c>
+      <c r="D28" s="8">
         <f t="shared" si="1"/>
-        <v>44641</v>
+        <v>44640</v>
       </c>
       <c r="F28" s="2"/>
       <c r="G28" s="2"/>
     </row>
     <row r="29" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>221</v>
-      </c>
-      <c r="D29" s="9">
+        <v>218</v>
+      </c>
+      <c r="D29" s="8">
         <f t="shared" si="1"/>
-        <v>44648</v>
+        <v>44647</v>
       </c>
       <c r="F29" s="2"/>
       <c r="G29" s="2"/>
     </row>
     <row r="30" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>222</v>
-      </c>
-      <c r="D30" s="9">
+        <v>219</v>
+      </c>
+      <c r="D30" s="8">
         <f t="shared" si="1"/>
-        <v>44655</v>
+        <v>44654</v>
       </c>
       <c r="F30" s="2"/>
       <c r="G30" s="2"/>
     </row>
     <row r="31" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>223</v>
-      </c>
-      <c r="D31" s="9">
+        <v>220</v>
+      </c>
+      <c r="D31" s="8">
         <f t="shared" si="1"/>
-        <v>44662</v>
+        <v>44661</v>
       </c>
       <c r="F31" s="2"/>
       <c r="G31" s="2"/>
     </row>
     <row r="32" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>224</v>
-      </c>
-      <c r="D32" s="9">
+        <v>221</v>
+      </c>
+      <c r="D32" s="8">
         <f t="shared" si="1"/>
-        <v>44669</v>
+        <v>44668</v>
       </c>
       <c r="F32" s="2"/>
       <c r="G32" s="2"/>
     </row>
     <row r="33" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="D33" s="9">
+        <v>222</v>
+      </c>
+      <c r="D33" s="8">
         <f t="shared" si="1"/>
-        <v>44676</v>
+        <v>44675</v>
       </c>
       <c r="F33" s="2"/>
       <c r="G33" s="2"/>
     </row>
     <row r="34" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>226</v>
-      </c>
-      <c r="D34" s="9">
+        <v>223</v>
+      </c>
+      <c r="D34" s="8">
         <f t="shared" si="1"/>
-        <v>44683</v>
+        <v>44682</v>
       </c>
       <c r="F34" s="2"/>
       <c r="G34" s="2"/>
     </row>
     <row r="35" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D35" s="9"/>
+      <c r="D35" s="8"/>
       <c r="F35" s="2"/>
       <c r="G35" s="2"/>
     </row>
     <row r="36" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>227</v>
-      </c>
-      <c r="D36" s="9">
+        <v>224</v>
+      </c>
+      <c r="D36" s="8">
         <v>44227</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D37" s="9"/>
+      <c r="D37" s="8"/>
     </row>
     <row r="38" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D38" s="9"/>
+      <c r="D38" s="8"/>
     </row>
     <row r="39" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>228</v>
-      </c>
-      <c r="D39" s="9">
+        <v>225</v>
+      </c>
+      <c r="D39" s="8">
         <v>44241</v>
       </c>
     </row>
     <row r="40" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D40" s="9"/>
+      <c r="D40" s="8"/>
     </row>
     <row r="41" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D41" s="9"/>
+      <c r="D41" s="8"/>
     </row>
     <row r="42" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
-        <v>229</v>
-      </c>
-      <c r="D42" s="9">
+        <v>226</v>
+      </c>
+      <c r="D42" s="8">
         <v>44262</v>
       </c>
     </row>
     <row r="43" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D43" s="9"/>
+      <c r="D43" s="8"/>
     </row>
     <row r="44" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D44" s="9"/>
+      <c r="D44" s="8"/>
     </row>
     <row r="45" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
-        <v>230</v>
-      </c>
-      <c r="D45" s="9">
+        <v>227</v>
+      </c>
+      <c r="D45" s="8">
         <v>44283</v>
       </c>
     </row>
     <row r="46" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D46" s="9"/>
+      <c r="D46" s="8"/>
     </row>
     <row r="47" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D47" s="9"/>
+      <c r="D47" s="8"/>
     </row>
     <row r="48" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>231</v>
-      </c>
-      <c r="D48" s="9">
+        <v>228</v>
+      </c>
+      <c r="D48" s="8">
         <v>44286</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D49" s="9"/>
+      <c r="D49" s="8"/>
     </row>
     <row r="50" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D50" s="9"/>
+      <c r="D50" s="8"/>
     </row>
     <row r="51" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
-        <v>232</v>
-      </c>
-      <c r="D51" s="9">
+        <v>229</v>
+      </c>
+      <c r="D51" s="8">
         <v>44267</v>
       </c>
     </row>
     <row r="52" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D52" s="9"/>
+      <c r="D52" s="8"/>
     </row>
     <row r="53" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D53" s="9"/>
+      <c r="D53" s="8"/>
     </row>
     <row r="54" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
-        <v>233</v>
-      </c>
-      <c r="D54" s="9">
+        <v>230</v>
+      </c>
+      <c r="D54" s="8">
         <v>44311</v>
       </c>
     </row>
     <row r="55" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D55" s="9"/>
+      <c r="D55" s="8"/>
     </row>
     <row r="56" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D56" s="9"/>
+      <c r="D56" s="8"/>
     </row>
     <row r="57" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D57" s="9"/>
+      <c r="D57" s="8"/>
     </row>
     <row r="58" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D58" s="9"/>
+      <c r="D58" s="8"/>
     </row>
     <row r="59" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D59" s="9"/>
+      <c r="D59" s="8"/>
     </row>
     <row r="60" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D60" s="9"/>
+      <c r="D60" s="8"/>
     </row>
     <row r="61" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D61" s="9"/>
+      <c r="D61" s="8"/>
     </row>
     <row r="62" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D62" s="9"/>
+      <c r="D62" s="8"/>
     </row>
     <row r="63" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D63" s="9"/>
+      <c r="D63" s="8"/>
     </row>
     <row r="64" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D64" s="9"/>
+      <c r="D64" s="8"/>
     </row>
     <row r="65" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D65" s="9"/>
+      <c r="D65" s="8"/>
     </row>
     <row r="66" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D66" s="9"/>
+      <c r="D66" s="8"/>
     </row>
     <row r="67" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D67" s="9"/>
+      <c r="D67" s="8"/>
     </row>
     <row r="68" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D68" s="9"/>
+      <c r="D68" s="8"/>
     </row>
     <row r="69" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D69" s="9"/>
+      <c r="D69" s="8"/>
     </row>
     <row r="70" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D70" s="9"/>
+      <c r="D70" s="8"/>
     </row>
     <row r="71" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D71" s="9"/>
+      <c r="D71" s="8"/>
     </row>
     <row r="72" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D72" s="9"/>
+      <c r="D72" s="8"/>
     </row>
     <row r="73" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D73" s="9"/>
+      <c r="D73" s="8"/>
     </row>
     <row r="74" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D74" s="9"/>
+      <c r="D74" s="8"/>
     </row>
     <row r="75" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D75" s="9"/>
+      <c r="D75" s="8"/>
     </row>
     <row r="76" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="77" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>